<commit_message>
addtion of concentration details
</commit_message>
<xml_diff>
--- a/KineticModel/gtoyall.xlsx
+++ b/KineticModel/gtoyall.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17030"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shyam\Documents\Courses\CHE1125Project\IntegratedModels\KineticModel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shyam\Documents\Courses\CHE1125Project\IntegratedModels\KineticModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,13 +13,14 @@
   </bookViews>
   <sheets>
     <sheet name="gtoy1" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="gtoy1C" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="97">
   <si>
     <t>Enzymes</t>
   </si>
@@ -324,6 +325,24 @@
   <si>
     <t>[c] : g6p &lt;==&gt; pep</t>
   </si>
+  <si>
+    <t>Mc (mM)</t>
+  </si>
+  <si>
+    <t>pyr[e]</t>
+  </si>
+  <si>
+    <t>pi[e]</t>
+  </si>
+  <si>
+    <t>ac[e]</t>
+  </si>
+  <si>
+    <t>g6p[e]</t>
+  </si>
+  <si>
+    <t>[c] : 1.496 3pg + 3.7478 accoa + 59.8100 atp + 0.3610 e4p + 0.0709 f6p + 0.1290 g3p + 0.2050 g6p + 59.8100 h2o + 3.5470 nad + 13.0279 nadph + 1.7867 oaa + 0.5191 pep + 2.8328 pyr + 0.8977 r5p --&gt; 59.8100 adp + 4.1182 akg + 3.7478 coa + 59.8100 h + 3.5470 nadh + 13.0279 nadp + 59.8100 pi</t>
+  </si>
 </sst>
 </file>
 
@@ -332,7 +351,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -379,6 +398,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -418,7 +445,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -430,6 +457,8 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -4224,6 +4253,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -4259,6 +4305,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4413,8 +4476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection sqref="A1:U15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4581,15 +4644,6 @@
       <c r="N4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="S4" t="s">
-        <v>52</v>
-      </c>
-      <c r="T4">
-        <v>0.27600000000000002</v>
-      </c>
-      <c r="U4">
-        <v>0.27600000000000002</v>
-      </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -4624,15 +4678,6 @@
       <c r="O5" t="s">
         <v>48</v>
       </c>
-      <c r="S5" t="s">
-        <v>49</v>
-      </c>
-      <c r="T5">
-        <v>0.111</v>
-      </c>
-      <c r="U5">
-        <v>0.111</v>
-      </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -4662,15 +4707,6 @@
       </c>
       <c r="O6" t="s">
         <v>23</v>
-      </c>
-      <c r="S6" t="s">
-        <v>24</v>
-      </c>
-      <c r="T6">
-        <v>3.48</v>
-      </c>
-      <c r="U6">
-        <v>3.48</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -4837,6 +4873,10 @@
         <v>-20</v>
       </c>
       <c r="N15" s="3"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="C16" s="12"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
@@ -4857,10 +4897,71 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U24"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection sqref="A1:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="6"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5586,7 +5687,13 @@
       </c>
       <c r="N24" s="3"/>
     </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C25" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
remove biomass reaction for testing
</commit_message>
<xml_diff>
--- a/KineticModel/gtoyall.xlsx
+++ b/KineticModel/gtoyall.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17030"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17030"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -4477,7 +4477,7 @@
   <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4960,8 +4960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
simiplified Kotte model for testing kientic model
</commit_message>
<xml_diff>
--- a/KineticModel/gtoyall.xlsx
+++ b/KineticModel/gtoyall.xlsx
@@ -9,16 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25590" windowHeight="7875"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25590" windowHeight="7875" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="gtoy1" sheetId="2" r:id="rId1"/>
     <sheet name="gtoy1C" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="gtoy2" sheetId="4" r:id="rId3"/>
+    <sheet name="gtoy2C" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <calcPr calcId="171027"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="116">
   <si>
     <t>Enzymes</t>
   </si>
@@ -342,6 +344,63 @@
   </si>
   <si>
     <t>[c] : 1.496 3pg + 3.7478 accoa + 59.8100 atp + 0.3610 e4p + 0.0709 f6p + 0.1290 g3p + 0.2050 g6p + 59.8100 h2o + 3.5470 nad + 13.0279 nadph + 1.7867 oaa + 0.5191 pep + 2.8328 pyr + 0.8977 r5p --&gt; 59.8100 adp + 4.1182 akg + 3.7478 coa + 59.8100 h + 3.5470 nadh + 13.0279 nadp + 59.8100 pi</t>
+  </si>
+  <si>
+    <t>ACpts</t>
+  </si>
+  <si>
+    <t>ac[e] ---&gt; pep[c]</t>
+  </si>
+  <si>
+    <t>0.1,0.1</t>
+  </si>
+  <si>
+    <t>glc[e]</t>
+  </si>
+  <si>
+    <t>GLUX</t>
+  </si>
+  <si>
+    <t>pep[c] ---&gt; fdp[c]</t>
+  </si>
+  <si>
+    <t>0.3,0.3</t>
+  </si>
+  <si>
+    <t>fdp[c] ---&gt; bm[c]</t>
+  </si>
+  <si>
+    <t>4 pep[c]</t>
+  </si>
+  <si>
+    <t>bmt2r</t>
+  </si>
+  <si>
+    <t>bm[c] ---&gt; bm[e]</t>
+  </si>
+  <si>
+    <t>PEPt2r</t>
+  </si>
+  <si>
+    <t>pep[c] ---&gt; pep[e]</t>
+  </si>
+  <si>
+    <t>PEPex</t>
+  </si>
+  <si>
+    <t>pep[e] &lt;==&gt;</t>
+  </si>
+  <si>
+    <t>bmex</t>
+  </si>
+  <si>
+    <t>bm[e] &lt;==&gt;</t>
+  </si>
+  <si>
+    <t>bm[e]</t>
+  </si>
+  <si>
+    <t>pep[e]</t>
   </si>
 </sst>
 </file>
@@ -445,7 +504,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -459,6 +518,15 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -4476,7 +4544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -4958,6 +5026,450 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U13"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection sqref="A1:U9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13">
+        <v>-30.5</v>
+      </c>
+      <c r="F2" s="13">
+        <v>-50.4</v>
+      </c>
+      <c r="G2" s="13">
+        <v>0.9</v>
+      </c>
+      <c r="H2" s="13"/>
+      <c r="I2" s="17">
+        <v>1</v>
+      </c>
+      <c r="J2" s="17">
+        <v>0</v>
+      </c>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13">
+        <v>1</v>
+      </c>
+      <c r="M2" s="18">
+        <v>14.285714285714301</v>
+      </c>
+      <c r="N2" s="16"/>
+      <c r="O2" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="T2" s="13">
+        <v>5.5599999999999997E-2</v>
+      </c>
+      <c r="U2" s="13">
+        <v>5.5599999999999997E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13">
+        <v>-30.5</v>
+      </c>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13">
+        <v>1</v>
+      </c>
+      <c r="J3" s="13">
+        <v>0</v>
+      </c>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13">
+        <v>1</v>
+      </c>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="13"/>
+      <c r="U3" s="13"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13">
+        <v>-30.5</v>
+      </c>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13">
+        <v>1</v>
+      </c>
+      <c r="J4" s="13">
+        <v>0</v>
+      </c>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13">
+        <v>1</v>
+      </c>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="P4" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="S4" s="13"/>
+      <c r="T4" s="13"/>
+      <c r="U4" s="13"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13">
+        <v>0</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13">
+        <v>1</v>
+      </c>
+      <c r="J5" s="13">
+        <v>1</v>
+      </c>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="13"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13">
+        <v>0</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13">
+        <v>1</v>
+      </c>
+      <c r="J6" s="13">
+        <v>1</v>
+      </c>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="13"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13">
+        <v>0</v>
+      </c>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13">
+        <v>1</v>
+      </c>
+      <c r="J7" s="13">
+        <v>1</v>
+      </c>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="13"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13">
+        <v>0</v>
+      </c>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13">
+        <v>1</v>
+      </c>
+      <c r="J8" s="13">
+        <v>1</v>
+      </c>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13">
+        <v>0</v>
+      </c>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="13"/>
+      <c r="S13" s="13"/>
+      <c r="T13" s="13"/>
+      <c r="U13" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="13">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">

</xml_diff>

<commit_message>
fixed Vmax for bmt2r = 1
</commit_message>
<xml_diff>
--- a/KineticModel/gtoyall.xlsx
+++ b/KineticModel/gtoyall.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17030"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -5285,7 +5285,9 @@
         <v>1</v>
       </c>
       <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
+      <c r="L6" s="13">
+        <v>1</v>
+      </c>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
       <c r="O6" s="13"/>

</xml_diff>

<commit_message>
new model file for extended model acetate
</commit_message>
<xml_diff>
--- a/KineticModel/gtoyall.xlsx
+++ b/KineticModel/gtoyall.xlsx
@@ -1,28 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shyam\Documents\Courses\CHE1125Project\IntegratedModels\KineticModel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shyam\Documents\Courses\CHE1125Project\IntegratedModels\KineticModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25590" windowHeight="7875" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25590" windowHeight="7875" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="gtoy1" sheetId="2" r:id="rId1"/>
     <sheet name="gtoy1C" sheetId="3" r:id="rId2"/>
     <sheet name="gtoy2" sheetId="4" r:id="rId3"/>
     <sheet name="gtoy2C" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId5"/>
+    <sheet name="gtoy3" sheetId="6" r:id="rId5"/>
+    <sheet name="gtoy3C" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
-    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
   </externalReferences>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="116">
   <si>
     <t>Enzymes</t>
   </si>
@@ -622,6 +624,7 @@
           <cell r="D3" t="str">
             <v>Transport, Extracellular</v>
           </cell>
+          <cell r="E3"/>
           <cell r="F3">
             <v>0</v>
           </cell>
@@ -735,6 +738,7 @@
           <cell r="D7" t="str">
             <v>Transport, Extracellular</v>
           </cell>
+          <cell r="E7"/>
           <cell r="F7">
             <v>0</v>
           </cell>
@@ -790,6 +794,7 @@
           <cell r="D9" t="str">
             <v>Citric Acid Cycle</v>
           </cell>
+          <cell r="E9"/>
           <cell r="F9">
             <v>-8.3000000000000007</v>
           </cell>
@@ -816,6 +821,7 @@
           <cell r="D10" t="str">
             <v>Transport, Extracellular</v>
           </cell>
+          <cell r="E10"/>
           <cell r="F10">
             <v>0</v>
           </cell>
@@ -871,6 +877,7 @@
           <cell r="D12" t="str">
             <v>Oxidative Phosphorylation</v>
           </cell>
+          <cell r="E12"/>
           <cell r="F12">
             <v>-6.6</v>
           </cell>
@@ -923,6 +930,10 @@
           <cell r="C14" t="str">
             <v>[c] : (1.496) 3pg + (3.7478) accoa + (59.8100) atp + (0.3610) e4p + (0.0709) f6p + (0.1290) g3p + (0.2050) g6p + (0.2557) gln-L + (4.9414) glu-L + (59.8100) h2o + (3.5470) nad + (13.0279) nadph + (1.7867) oaa + (0.5191) pep + (2.8328) pyr + (0.8977) r5p --&gt; (59.8100) adp + (4.1182) akg + (3.7478) coa + (59.8100) h + (3.5470) nadh + (13.0279) nadp + (59.8100) pi</v>
           </cell>
+          <cell r="D14"/>
+          <cell r="E14"/>
+          <cell r="F14"/>
+          <cell r="G14"/>
           <cell r="H14">
             <v>0.87390000000000001</v>
           </cell>
@@ -943,6 +954,7 @@
           <cell r="D15" t="str">
             <v>Transport, Extracellular</v>
           </cell>
+          <cell r="E15"/>
           <cell r="F15">
             <v>0</v>
           </cell>
@@ -969,6 +981,7 @@
           <cell r="D16" t="str">
             <v>Citric Acid Cycle</v>
           </cell>
+          <cell r="E16"/>
           <cell r="F16">
             <v>-8.6</v>
           </cell>
@@ -995,6 +1008,7 @@
           <cell r="D17" t="str">
             <v>Oxidative Phosphorylation</v>
           </cell>
+          <cell r="E17"/>
           <cell r="F17">
             <v>-37.200000000000003</v>
           </cell>
@@ -1021,6 +1035,7 @@
           <cell r="D18" t="str">
             <v>Transport, Extracellular</v>
           </cell>
+          <cell r="E18"/>
           <cell r="F18">
             <v>0</v>
           </cell>
@@ -1076,6 +1091,7 @@
           <cell r="D20" t="str">
             <v>Transport, Extracellular</v>
           </cell>
+          <cell r="E20"/>
           <cell r="F20">
             <v>0</v>
           </cell>
@@ -1102,6 +1118,9 @@
           <cell r="D21" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E21"/>
+          <cell r="F21"/>
+          <cell r="G21"/>
           <cell r="H21">
             <v>0</v>
           </cell>
@@ -1122,6 +1141,9 @@
           <cell r="D22" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E22"/>
+          <cell r="F22"/>
+          <cell r="G22"/>
           <cell r="H22">
             <v>0</v>
           </cell>
@@ -1142,6 +1164,9 @@
           <cell r="D23" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E23"/>
+          <cell r="F23"/>
+          <cell r="G23"/>
           <cell r="H23">
             <v>0</v>
           </cell>
@@ -1162,6 +1187,9 @@
           <cell r="D24" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E24"/>
+          <cell r="F24"/>
+          <cell r="G24"/>
           <cell r="H24">
             <v>22.809799999999999</v>
           </cell>
@@ -1182,6 +1210,9 @@
           <cell r="D25" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E25"/>
+          <cell r="F25"/>
+          <cell r="G25"/>
           <cell r="H25">
             <v>0</v>
           </cell>
@@ -1202,6 +1233,9 @@
           <cell r="D26" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E26"/>
+          <cell r="F26"/>
+          <cell r="G26"/>
           <cell r="H26">
             <v>0</v>
           </cell>
@@ -1222,6 +1256,9 @@
           <cell r="D27" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E27"/>
+          <cell r="F27"/>
+          <cell r="G27"/>
           <cell r="H27">
             <v>0</v>
           </cell>
@@ -1242,6 +1279,9 @@
           <cell r="D28" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E28"/>
+          <cell r="F28"/>
+          <cell r="G28"/>
           <cell r="H28">
             <v>0</v>
           </cell>
@@ -1262,6 +1302,9 @@
           <cell r="D29" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E29"/>
+          <cell r="F29"/>
+          <cell r="G29"/>
           <cell r="H29">
             <v>-10</v>
           </cell>
@@ -1282,6 +1325,9 @@
           <cell r="D30" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E30"/>
+          <cell r="F30"/>
+          <cell r="G30"/>
           <cell r="H30">
             <v>0</v>
           </cell>
@@ -1302,6 +1348,9 @@
           <cell r="D31" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E31"/>
+          <cell r="F31"/>
+          <cell r="G31"/>
           <cell r="H31">
             <v>0</v>
           </cell>
@@ -1322,6 +1371,9 @@
           <cell r="D32" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E32"/>
+          <cell r="F32"/>
+          <cell r="G32"/>
           <cell r="H32">
             <v>17.530899999999999</v>
           </cell>
@@ -1342,6 +1394,9 @@
           <cell r="D33" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E33"/>
+          <cell r="F33"/>
+          <cell r="G33"/>
           <cell r="H33">
             <v>29.175799999999999</v>
           </cell>
@@ -1362,6 +1417,9 @@
           <cell r="D34" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E34"/>
+          <cell r="F34"/>
+          <cell r="G34"/>
           <cell r="H34">
             <v>0</v>
           </cell>
@@ -1382,6 +1440,9 @@
           <cell r="D35" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E35"/>
+          <cell r="F35"/>
+          <cell r="G35"/>
           <cell r="H35">
             <v>0</v>
           </cell>
@@ -1402,6 +1463,9 @@
           <cell r="D36" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E36"/>
+          <cell r="F36"/>
+          <cell r="G36"/>
           <cell r="H36">
             <v>-4.7652999999999999</v>
           </cell>
@@ -1422,6 +1486,9 @@
           <cell r="D37" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E37"/>
+          <cell r="F37"/>
+          <cell r="G37"/>
           <cell r="H37">
             <v>-21.799499999999998</v>
           </cell>
@@ -1442,6 +1509,9 @@
           <cell r="D38" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E38"/>
+          <cell r="F38"/>
+          <cell r="G38"/>
           <cell r="H38">
             <v>-3.2149000000000001</v>
           </cell>
@@ -1462,6 +1532,9 @@
           <cell r="D39" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E39"/>
+          <cell r="F39"/>
+          <cell r="G39"/>
           <cell r="H39">
             <v>0</v>
           </cell>
@@ -1482,6 +1555,9 @@
           <cell r="D40" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E40"/>
+          <cell r="F40"/>
+          <cell r="G40"/>
           <cell r="H40">
             <v>0</v>
           </cell>
@@ -1560,6 +1636,7 @@
           <cell r="D43" t="str">
             <v>Transport, Extracellular</v>
           </cell>
+          <cell r="E43"/>
           <cell r="F43">
             <v>0</v>
           </cell>
@@ -1586,6 +1663,7 @@
           <cell r="D44" t="str">
             <v>Transport, Extracellular</v>
           </cell>
+          <cell r="E44"/>
           <cell r="F44">
             <v>0</v>
           </cell>
@@ -1641,6 +1719,7 @@
           <cell r="D46" t="str">
             <v>Transport, Extracellular</v>
           </cell>
+          <cell r="E46"/>
           <cell r="F46">
             <v>-9.1</v>
           </cell>
@@ -1696,6 +1775,7 @@
           <cell r="D48" t="str">
             <v>Transport, Extracellular</v>
           </cell>
+          <cell r="E48"/>
           <cell r="F48">
             <v>0</v>
           </cell>
@@ -1780,6 +1860,7 @@
           <cell r="D51" t="str">
             <v>Transport, Extracellular</v>
           </cell>
+          <cell r="E51"/>
           <cell r="F51">
             <v>-9.1</v>
           </cell>
@@ -1835,6 +1916,7 @@
           <cell r="D53" t="str">
             <v>Transport, Extracellular</v>
           </cell>
+          <cell r="E53"/>
           <cell r="F53">
             <v>-6.6</v>
           </cell>
@@ -1948,6 +2030,7 @@
           <cell r="D57" t="str">
             <v>Transport, Extracellular</v>
           </cell>
+          <cell r="E57"/>
           <cell r="F57">
             <v>0</v>
           </cell>
@@ -2003,6 +2086,7 @@
           <cell r="D59" t="str">
             <v>Transport, Extracellular</v>
           </cell>
+          <cell r="E59"/>
           <cell r="F59">
             <v>0</v>
           </cell>
@@ -2145,6 +2229,7 @@
           <cell r="D64" t="str">
             <v>Transport, Extracellular</v>
           </cell>
+          <cell r="E64"/>
           <cell r="F64">
             <v>0</v>
           </cell>
@@ -2316,6 +2401,7 @@
           <cell r="D70" t="str">
             <v>Inorganic Ion Transport and Metabolism</v>
           </cell>
+          <cell r="E70"/>
           <cell r="F70">
             <v>0</v>
           </cell>
@@ -2342,6 +2428,7 @@
           <cell r="D71" t="str">
             <v>Transport, Extracellular</v>
           </cell>
+          <cell r="E71"/>
           <cell r="F71">
             <v>0</v>
           </cell>
@@ -2368,6 +2455,7 @@
           <cell r="D72" t="str">
             <v>Glycolysis/Gluconeogenesis</v>
           </cell>
+          <cell r="E72"/>
           <cell r="F72">
             <v>-8.3000000000000007</v>
           </cell>
@@ -2423,6 +2511,7 @@
           <cell r="D74" t="str">
             <v>Pyruvate Metabolism</v>
           </cell>
+          <cell r="E74"/>
           <cell r="F74">
             <v>-5.0999999999999996</v>
           </cell>
@@ -2565,6 +2654,7 @@
           <cell r="D79" t="str">
             <v>Inorganic Ion Transport and Metabolism</v>
           </cell>
+          <cell r="E79"/>
           <cell r="F79">
             <v>0</v>
           </cell>
@@ -4321,23 +4411,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -4373,23 +4446,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5028,7 +5084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:U9"/>
     </sheetView>
   </sheetViews>
@@ -5427,6 +5483,550 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="13">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="34" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="13">
+        <f>VLOOKUP(A2,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="17">
+        <v>1</v>
+      </c>
+      <c r="J2" s="13">
+        <v>1</v>
+      </c>
+      <c r="M2" s="18">
+        <v>-19.215657194822899</v>
+      </c>
+      <c r="N2" s="16"/>
+      <c r="O2" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13">
+        <v>-30.5</v>
+      </c>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13">
+        <v>1</v>
+      </c>
+      <c r="J3" s="13">
+        <v>0</v>
+      </c>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13">
+        <v>1</v>
+      </c>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="13"/>
+      <c r="U3" s="13"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13">
+        <v>-30.5</v>
+      </c>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13">
+        <v>1</v>
+      </c>
+      <c r="J4" s="13">
+        <v>0</v>
+      </c>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13">
+        <v>1</v>
+      </c>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="P4" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="S4" s="13"/>
+      <c r="T4" s="13"/>
+      <c r="U4" s="13"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13">
+        <v>0</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13">
+        <v>1</v>
+      </c>
+      <c r="J5" s="13">
+        <v>1</v>
+      </c>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="13"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13">
+        <v>0</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13">
+        <v>1</v>
+      </c>
+      <c r="J6" s="13">
+        <v>1</v>
+      </c>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13">
+        <v>1</v>
+      </c>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="13"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13">
+        <v>0</v>
+      </c>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13">
+        <v>1</v>
+      </c>
+      <c r="J7" s="13">
+        <v>1</v>
+      </c>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="13"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13">
+        <v>0</v>
+      </c>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13">
+        <v>1</v>
+      </c>
+      <c r="J8" s="13">
+        <v>1</v>
+      </c>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13">
+        <v>0</v>
+      </c>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13"/>
+    </row>
+    <row r="10" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="13">
+        <f>VLOOKUP(A10,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>4.3</v>
+      </c>
+      <c r="F10" s="13">
+        <v>-24.3</v>
+      </c>
+      <c r="G10" s="13">
+        <v>52.1</v>
+      </c>
+      <c r="I10" s="13">
+        <v>280</v>
+      </c>
+      <c r="M10" s="18">
+        <v>-19.215657194822899</v>
+      </c>
+      <c r="N10" s="16" t="str">
+        <f>VLOOKUP(A10,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.7.2.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="13">
+        <f>VLOOKUP(A11,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>3.8</v>
+      </c>
+      <c r="F11" s="13">
+        <v>-20.399999999999999</v>
+      </c>
+      <c r="G11" s="13">
+        <v>28.7</v>
+      </c>
+      <c r="I11" s="13">
+        <v>120</v>
+      </c>
+      <c r="J11" s="13">
+        <v>0.02</v>
+      </c>
+      <c r="M11" s="7">
+        <v>19.215657194822899</v>
+      </c>
+      <c r="N11" s="16" t="str">
+        <f>VLOOKUP(A11,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.3.1.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="13">
+        <v>-8.3000000000000007</v>
+      </c>
+      <c r="F12" s="13">
+        <v>-73</v>
+      </c>
+      <c r="G12" s="13">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I12" s="13">
+        <v>6.32</v>
+      </c>
+      <c r="M12" s="18">
+        <v>0</v>
+      </c>
+      <c r="N12" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="S12" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="T12" s="13">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="U12" s="13">
+        <v>0.27600000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="13">
+        <v>-31.12</v>
+      </c>
+      <c r="F13" s="13">
+        <v>-10.8</v>
+      </c>
+      <c r="G13" s="13">
+        <v>65.3</v>
+      </c>
+      <c r="H13" s="20"/>
+      <c r="I13" s="13">
+        <v>2540</v>
+      </c>
+      <c r="M13" s="18">
+        <v>-8.5077261088811902</v>
+      </c>
+      <c r="N13" s="16" t="str">
+        <f>VLOOKUP(A13,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.7.1.40</v>
+      </c>
+      <c r="O13" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="S13" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="T13" s="13">
+        <v>0.111</v>
+      </c>
+      <c r="U13" s="13">
+        <v>0.111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B4"/>
     </sheetView>
@@ -5470,12 +6070,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U25"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>